<commit_message>
Removed correlated from test files. ASK-85
</commit_message>
<xml_diff>
--- a/test/Assembly.Kernel.Acceptance.Test/test-data/definitions/Benchmarktest_traject 12-2.xlsx
+++ b/test/Assembly.Kernel.Acceptance.Test/test-data/definitions/Benchmarktest_traject 12-2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Projects\11209000\11209269\B. Measurements and calculations\007 Assemblagekernel\Testcases\Aangepast\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Checkouts\AssemblageKernel\test\Assembly.Kernel.Acceptance.Test\test-data\definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A636FA3-612D-447B-9B5A-3AAF29282D49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB961299-F5C3-447E-B90E-86BA14C9A87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="9" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="9" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -2188,7 +2188,7 @@
   <dimension ref="B2:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D3"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="D2" s="1">
         <f>IFERROR(1-PRODUCT(M7:M13)*(1-L15),"GR")</f>
-        <v>6.0686442949805408E-2</v>
+        <v>6.0686446349930367E-2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(D2="GR","-",INDEX('Normen en duidingsklassen'!$D$4:$D$8,I2))</f>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="D3" s="1">
         <f>1-PRODUCT(O7:O13)*(1-N15)</f>
-        <v>6.0686442949805408E-2</v>
+        <v>6.0686446349930367E-2</v>
       </c>
       <c r="E3" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$4:$D$8,I3)</f>
@@ -2311,11 +2311,11 @@
         <v>0</v>
       </c>
       <c r="H7" s="1">
-        <f>IF(ISNUMBER(E7),1-E7,1-C7)</f>
+        <f t="shared" ref="H7:H13" si="0">IF(ISNUMBER(E7),1-E7,1-C7)</f>
         <v>0.93933311356008209</v>
       </c>
       <c r="I7" s="1">
-        <f>IF(ISNUMBER(E7),1-E7,1-D7)</f>
+        <f t="shared" ref="I7:I13" si="1">IF(ISNUMBER(E7),1-E7,1-D7)</f>
         <v>0.93933311356008209</v>
       </c>
       <c r="J7" s="1">
@@ -2327,7 +2327,7 @@
         <v>6.0666886439917911E-2</v>
       </c>
       <c r="L7" s="1">
-        <f>F7*J7</f>
+        <f t="shared" ref="L7:L13" si="2">F7*J7</f>
         <v>0</v>
       </c>
       <c r="M7" s="1">
@@ -2335,7 +2335,7 @@
         <v>0.93933311356008209</v>
       </c>
       <c r="N7" s="1">
-        <f>F7*K7</f>
+        <f t="shared" ref="N7:N13" si="3">F7*K7</f>
         <v>0</v>
       </c>
       <c r="O7" s="1">
@@ -2360,35 +2360,35 @@
         <v>0</v>
       </c>
       <c r="H8" s="1">
-        <f>IF(ISNUMBER(E8),1-E8,1-C8)</f>
+        <f t="shared" si="0"/>
         <v>0.99999625083543664</v>
       </c>
       <c r="I8" s="1">
-        <f>IF(ISNUMBER(E8),1-E8,1-D8)</f>
+        <f t="shared" si="1"/>
         <v>0.99999625083543664</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" ref="J8:J13" si="0">1-H8</f>
+        <f t="shared" ref="J8:J13" si="4">1-H8</f>
         <v>3.7491645633602744E-6</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" ref="K8:K13" si="1">1-I8</f>
+        <f t="shared" ref="K8:K13" si="5">1-I8</f>
         <v>3.7491645633602744E-6</v>
       </c>
       <c r="L8" s="1">
-        <f>F8*J8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" ref="M8:M13" si="2">1-(1-F8)*J8</f>
+        <f t="shared" ref="M8:M13" si="6">1-(1-F8)*J8</f>
         <v>0.99999625083543664</v>
       </c>
       <c r="N8" s="1">
-        <f>F8*K8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" ref="O8:O13" si="3">1-(1-F8)*K8</f>
+        <f t="shared" ref="O8:O13" si="7">1-(1-F8)*K8</f>
         <v>0.99999625083543664</v>
       </c>
     </row>
@@ -2406,39 +2406,39 @@
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="1">
-        <f>IF(ISNUMBER(E9),1-E9,1-C9)</f>
+        <f t="shared" si="0"/>
         <v>0.99999554325999995</v>
       </c>
       <c r="I9" s="1">
-        <f>IF(ISNUMBER(E9),1-E9,1-D9)</f>
+        <f t="shared" si="1"/>
         <v>0.99999554325999995</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>4.4567400000472546E-6</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4.4567400000472546E-6</v>
       </c>
       <c r="L9" s="1">
-        <f>F9*J9</f>
-        <v>4.4567400000472546E-6</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="M9" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.99999554325999995</v>
       </c>
       <c r="N9" s="1">
-        <f>F9*K9</f>
-        <v>4.4567400000472546E-6</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O9" s="1">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>0.99999554325999995</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -2458,35 +2458,35 @@
         <v>0</v>
       </c>
       <c r="H10" s="1">
-        <f>IF(ISNUMBER(E10),1-E10,1-C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I10" s="1">
-        <f>IF(ISNUMBER(E10),1-E10,1-D10)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="L10" s="1">
-        <f>F10*J10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="N10" s="1">
-        <f>F10*K10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
     </row>
@@ -2507,35 +2507,35 @@
         <v>0</v>
       </c>
       <c r="H11" s="1">
-        <f>IF(ISNUMBER(E11),1-E11,1-C11)</f>
+        <f t="shared" si="0"/>
         <v>0.9999886413605209</v>
       </c>
       <c r="I11" s="1">
-        <f>IF(ISNUMBER(E11),1-E11,1-D11)</f>
+        <f t="shared" si="1"/>
         <v>0.9999886413605209</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.1358639479097654E-5</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.1358639479097654E-5</v>
       </c>
       <c r="L11" s="1">
-        <f>F11*J11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.9999886413605209</v>
       </c>
       <c r="N11" s="1">
-        <f>F11*K11</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.9999886413605209</v>
       </c>
     </row>
@@ -2553,39 +2553,39 @@
       </c>
       <c r="E12" s="49"/>
       <c r="F12" s="23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="1">
-        <f>IF(ISNUMBER(E12),1-E12,1-C12)</f>
+        <f t="shared" si="0"/>
         <v>0.99999999638020232</v>
       </c>
       <c r="I12" s="1">
-        <f>IF(ISNUMBER(E12),1-E12,1-D12)</f>
+        <f t="shared" si="1"/>
         <v>0.99999999638020232</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>3.6197976838181489E-9</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3.6197976838181489E-9</v>
       </c>
       <c r="L12" s="1">
-        <f>F12*J12</f>
-        <v>3.6197976838181489E-9</v>
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
       <c r="M12" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="6"/>
+        <v>0.99999999638020232</v>
       </c>
       <c r="N12" s="1">
-        <f>F12*K12</f>
-        <v>3.6197976838181489E-9</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="O12" s="1">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>0.99999999638020232</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -2605,35 +2605,35 @@
         <v>0</v>
       </c>
       <c r="H13" s="1">
-        <f>IF(ISNUMBER(E13),1-E13,1-C13)</f>
+        <f t="shared" si="0"/>
         <v>0.99999874484129769</v>
       </c>
       <c r="I13" s="1">
-        <f>IF(ISNUMBER(E13),1-E13,1-D13)</f>
+        <f t="shared" si="1"/>
         <v>0.99999874484129769</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>1.2551587023068578E-6</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1.2551587023068578E-6</v>
       </c>
       <c r="L13" s="1">
-        <f>F13*J13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>0.99999874484129769</v>
       </c>
       <c r="N13" s="1">
-        <f>F13*K13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="O13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0.99999874484129769</v>
       </c>
     </row>
@@ -2655,11 +2655,11 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1">
         <f>MAX(L7:L13)</f>
-        <v>4.4567400000472546E-6</v>
+        <v>0</v>
       </c>
       <c r="N15" s="1">
         <f>MAX(N7:N13)</f>
-        <v>4.4567400000472546E-6</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated acceptance test files. ASK-87
</commit_message>
<xml_diff>
--- a/test/Assembly.Kernel.Acceptance.Test/test-data/definitions/Benchmarktest_traject 12-2.xlsx
+++ b/test/Assembly.Kernel.Acceptance.Test/test-data/definitions/Benchmarktest_traject 12-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Checkouts\AssemblageKernel\test\Assembly.Kernel.Acceptance.Test\test-data\definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB961299-F5C3-447E-B90E-86BA14C9A87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7B0C2D-3DCE-4954-BB81-4632A2E6BC7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" firstSheet="1" activeTab="9" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
@@ -2188,7 +2188,7 @@
   <dimension ref="B2:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="F7" sqref="F7:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2213,7 +2213,7 @@
       </c>
       <c r="D2" s="1">
         <f>IFERROR(1-PRODUCT(M7:M13)*(1-L15),"GR")</f>
-        <v>6.0686446349930367E-2</v>
+        <v>6.0686442949805408E-2</v>
       </c>
       <c r="E2" t="str">
         <f>IF(D2="GR","-",INDEX('Normen en duidingsklassen'!$D$4:$D$8,I2))</f>
@@ -2234,7 +2234,7 @@
       </c>
       <c r="D3" s="1">
         <f>1-PRODUCT(O7:O13)*(1-N15)</f>
-        <v>6.0686446349930367E-2</v>
+        <v>6.0686442949805408E-2</v>
       </c>
       <c r="E3" t="str">
         <f>INDEX('Normen en duidingsklassen'!$D$4:$D$8,I3)</f>
@@ -2406,7 +2406,7 @@
       </c>
       <c r="E9" s="49"/>
       <c r="F9" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="0"/>
@@ -2426,19 +2426,19 @@
       </c>
       <c r="L9" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.4567400000472546E-6</v>
       </c>
       <c r="M9" s="1">
         <f t="shared" si="6"/>
-        <v>0.99999554325999995</v>
+        <v>1</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.4567400000472546E-6</v>
       </c>
       <c r="O9" s="1">
         <f t="shared" si="7"/>
-        <v>0.99999554325999995</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
@@ -2553,7 +2553,7 @@
       </c>
       <c r="E12" s="49"/>
       <c r="F12" s="23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="0"/>
@@ -2573,19 +2573,19 @@
       </c>
       <c r="L12" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3.6197976838181489E-9</v>
       </c>
       <c r="M12" s="1">
         <f t="shared" si="6"/>
-        <v>0.99999999638020232</v>
+        <v>1</v>
       </c>
       <c r="N12" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>3.6197976838181489E-9</v>
       </c>
       <c r="O12" s="1">
         <f t="shared" si="7"/>
-        <v>0.99999999638020232</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.25">
@@ -2655,11 +2655,11 @@
       <c r="K15" s="1"/>
       <c r="L15" s="1">
         <f>MAX(L7:L13)</f>
-        <v>0</v>
+        <v>4.4567400000472546E-6</v>
       </c>
       <c r="N15" s="1">
         <f>MAX(N7:N13)</f>
-        <v>0</v>
+        <v>4.4567400000472546E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>